<commit_message>
#main update data employee
</commit_message>
<xml_diff>
--- a/data/Models/Employee.xlsx
+++ b/data/Models/Employee.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -109,15 +109,6 @@
   </si>
   <si>
     <t>jha@gmail.com</t>
-  </si>
-  <si>
-    <t>data/face_train/TrungTQ4/2021-05-11-16-43-57-991777.jpg</t>
-  </si>
-  <si>
-    <t>data/face_train/TrungTQ2/2021-05-11-16-49-05-335656.jpg</t>
-  </si>
-  <si>
-    <t>data/face_train/TrungTQ4/2021-05-11-16-43-59-380232.jpg</t>
   </si>
 </sst>
 </file>
@@ -492,12 +483,14 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -587,9 +580,6 @@
       <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -624,9 +614,6 @@
       <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -661,9 +648,6 @@
       <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -680,9 +664,6 @@
       </c>
       <c r="E10" t="s">
         <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#main apply checkin checkout
</commit_message>
<xml_diff>
--- a/data/Models/Employee.xlsx
+++ b/data/Models/Employee.xlsx
@@ -42,25 +42,25 @@
     <t>QuangHD</t>
   </si>
   <si>
-    <t>NganLNT</t>
+    <t>QuangTrung</t>
   </si>
   <si>
     <t>Hồ Duy Quang</t>
   </si>
   <si>
-    <t>Lý Ngọc Thu Ngân</t>
+    <t>Trần Quang Trung</t>
   </si>
   <si>
     <t>hoduyquang@gmail.com</t>
   </si>
   <si>
-    <t>lyngocthungan@gmail.com</t>
-  </si>
-  <si>
-    <t>data/face_train/QuangHD/2021-05-15-03-18-46-389227.jpg</t>
-  </si>
-  <si>
-    <t>data/face_train/NganLNT/2021-05-15-03-39-07-182901.jpg</t>
+    <t>quangtrung@gmail.com</t>
+  </si>
+  <si>
+    <t>data/face_train/QuangTrung/2021-05-17-14-12-56-012379.jpg</t>
+  </si>
+  <si>
+    <t>sdafdsafasdfsad</t>
   </si>
 </sst>
 </file>
@@ -432,16 +432,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="51" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -480,7 +477,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -500,29 +497,8 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D10" s="2"/>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#main fix update employee
</commit_message>
<xml_diff>
--- a/data/Models/Employee.xlsx
+++ b/data/Models/Employee.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\time-attendance-by-face-recognition\data\Models\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -42,7 +37,7 @@
     <t>QuangHD</t>
   </si>
   <si>
-    <t>QuangTrung</t>
+    <t>TrungTQ</t>
   </si>
   <si>
     <t>Hồ Duy Quang</t>
@@ -58,19 +53,17 @@
   </si>
   <si>
     <t>data/face_train/QuangTrung/2021-05-17-14-12-56-012379.jpg</t>
-  </si>
-  <si>
-    <t>sdafdsafasdfsad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,26 +115,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -188,7 +174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,10 +206,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,7 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -431,16 +415,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -476,11 +458,8 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -490,7 +469,7 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>36271</v>
       </c>
       <c r="E3" t="s">

</xml_diff>